<commit_message>
allow user to enter dataset title on upload, changes to users dataset list
</commit_message>
<xml_diff>
--- a/public/templates/edna_template.xlsx
+++ b/public/templates/edna_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vgs417/edna-tool-ui/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF077FC-825B-0B43-99BB-1ED5CA8D8339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE23CD8-2932-614D-B139-2BB3EF278456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45900" yWindow="-19100" windowWidth="34540" windowHeight="18840" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17680" activeTab="3" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
   </bookViews>
   <sheets>
     <sheet name="OTU_table" sheetId="1" r:id="rId1"/>
     <sheet name="taxon" sheetId="2" r:id="rId2"/>
     <sheet name="sample" sheetId="3" r:id="rId3"/>
-    <sheet name="study" sheetId="4" r:id="rId4"/>
+    <sheet name="defaultValues" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C892BD8-C93C-C74D-A89F-6FFFFFF15579}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73708D4D-E6C2-A347-9F42-4980BDC24EB9}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
when Jaccard return undefined for empty sets, use 0 as value
</commit_message>
<xml_diff>
--- a/public/templates/edna_template.xlsx
+++ b/public/templates/edna_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vgs417/edna-tool-ui/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE23CD8-2932-614D-B139-2BB3EF278456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0716CD78-9E2C-0643-B3DC-5D164FA36411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17680" activeTab="3" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
+    <workbookView xWindow="42000" yWindow="-9760" windowWidth="29920" windowHeight="17680" activeTab="2" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
   </bookViews>
   <sheets>
     <sheet name="OTU_table" sheetId="1" r:id="rId1"/>
@@ -231,6 +231,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -262,7 +265,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,7 +823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2128B45-DA79-B649-82CD-21102A8D0AD4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -907,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73708D4D-E6C2-A347-9F42-4980BDC24EB9}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some content on how to use page, check that sequence, eventDate and lat lon exists when user leaves mapping
</commit_message>
<xml_diff>
--- a/public/templates/edna_template.xlsx
+++ b/public/templates/edna_template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vgs417/edna-tool-ui/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0716CD78-9E2C-0643-B3DC-5D164FA36411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A98C229-A47B-424B-94C1-86C968B8B63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42000" yWindow="-9760" windowWidth="29920" windowHeight="17680" activeTab="2" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
+    <workbookView xWindow="43920" yWindow="-16260" windowWidth="29920" windowHeight="18660" xr2:uid="{A71D9F63-A05D-0B42-B9B0-1902D799A659}"/>
   </bookViews>
   <sheets>
     <sheet name="OTU_table" sheetId="1" r:id="rId1"/>
     <sheet name="taxon" sheetId="2" r:id="rId2"/>
     <sheet name="sample" sheetId="3" r:id="rId3"/>
     <sheet name="defaultValues" sheetId="4" r:id="rId4"/>
+    <sheet name="ReadMe" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -225,6 +226,120 @@
   </si>
   <si>
     <t>UNITE v9.3</t>
+  </si>
+  <si>
+    <t>This sheet should contain the read counts of OTUs in samples</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
+  </si>
+  <si>
+    <t>Keep readcounts as they are. Do not transform into relative abundance or rarefy/resample</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>OTU_table sheet</t>
+  </si>
+  <si>
+    <t>Remember to remove the row with column sums if you have one</t>
+  </si>
+  <si>
+    <t>OTU IDs should be unique. Only OTU Ids that are also present in the OTU table (OR in a separate fasta file with sequences) will be processed</t>
+  </si>
+  <si>
+    <t>Unite SH numbers can be used as ScientifiName</t>
+  </si>
+  <si>
+    <t>BOLD BIN numbers can be used as ScientificName</t>
+  </si>
+  <si>
+    <t>This sheet should contain all information associated with the sample</t>
+  </si>
+  <si>
+    <t>Sample IDs should be unique. Only Sample IDs that are also present in the OTU_table sheet will be processed</t>
+  </si>
+  <si>
+    <t>Sample IDs should be unique. Only Sample Ids that are also present in the sample sheet will be processed</t>
+  </si>
+  <si>
+    <t>This ReadMe relates only to cases where you intend to use this excel template for the GBIF eDNA tool. You can also use the tool with TSV (txt) files. See elsewhere for instructions on that.</t>
+  </si>
+  <si>
+    <t>Location of the sample should be given as decimal degrees in the two fields decimalLatitude and decimalLongitude</t>
+  </si>
+  <si>
+    <t>OTU IDs should be unique. Only OTU Ids that are also present in the taxon sheet (OR in a separate fasta file with sequences) will be processed</t>
+  </si>
+  <si>
+    <t>This sheet should contain all information associated with each OTU.</t>
+  </si>
+  <si>
+    <t>The sequence of the ASV/OTU should be put into the field DNA_sequence (unless a separate fasta file with sequences is supplied)</t>
+  </si>
+  <si>
+    <t>GBIF understands the taxonomic ranks Kingdom, Phylum, Class, Order, Family, Genus and ScientificName.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you assigned taxonomy to your sequences, you should provide that.   Kingdom and ScientificName is often enough for the interpretation </t>
+  </si>
+  <si>
+    <t>Scientific name should be the finest taxonomic level possible to identify (often species).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All OTUs/ASVs are likely produced with the same set of primers and in the same sequencing run. </t>
+  </si>
+  <si>
+    <t>Information relating to this, can then be provided as universal values in the DefaultValues sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have combined OTUs from different primer sets in the same table, you need to provide information on primers, etc in this sheet for each ASV/OTU. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We recommend splitting into datasets that each reflect all result based on one  primerset (and using the same lab setups) for interoperability purposes </t>
+  </si>
+  <si>
+    <t>Sampling date should be provided in eventDate</t>
+  </si>
+  <si>
+    <t>We recommend to fill in as many fields from the MiXS standard as you can to describe you samples well</t>
+  </si>
+  <si>
+    <t>We recommend to fill in as many fields from the MiXS standard as you can to describe you PCR, sequencing and bioinformatics well</t>
+  </si>
+  <si>
+    <t>Most likely this can be done as default values (see below)</t>
+  </si>
+  <si>
+    <t>defaultValues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet accepts universal/default values that apply to all samples and ASVs/OTUs in the dataset. All MiXS terms are accepted, along with </t>
+  </si>
+  <si>
+    <t>You need to set your default values by putting the term name of the standard DarwnCore field in the term column and the corresponding universal value for you dataset in the value field</t>
+  </si>
+  <si>
+    <t>Some terms use a fixed vocabulary (see below)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will often be able to put most of the relevant information here. </t>
+  </si>
+  <si>
+    <t>Tips/notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxon sheet </t>
+  </si>
+  <si>
+    <t>sample sheet</t>
+  </si>
+  <si>
+    <t>All terms from https://rs.gbif.org/core/dwc_occurrence_2022-02-02.xml and https://rs.gbif.org/extension/gbif/1.0/dna_derived_data_2022-02-23.xml wil be accepted</t>
   </si>
 </sst>
 </file>
@@ -232,7 +347,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -243,12 +358,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,9 +384,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +704,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C892BD8-C93C-C74D-A89F-6FFFFFF15579}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="B2:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -823,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2128B45-DA79-B649-82CD-21102A8D0AD4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
@@ -857,7 +981,7 @@
       <c r="C2">
         <v>10.363237639336299</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>41960</v>
       </c>
     </row>
@@ -871,7 +995,7 @@
       <c r="C3">
         <v>10.0780350249746</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>41961</v>
       </c>
     </row>
@@ -885,7 +1009,7 @@
       <c r="C4">
         <v>10.404033328091799</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>41960</v>
       </c>
     </row>
@@ -899,7 +1023,7 @@
       <c r="C5">
         <v>9.9261798517494508</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>41961</v>
       </c>
     </row>
@@ -913,7 +1037,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,7 +1058,7 @@
       <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -942,7 +1066,7 @@
       <c r="A3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -950,7 +1074,7 @@
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -958,7 +1082,7 @@
       <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -966,7 +1090,7 @@
       <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -974,7 +1098,7 @@
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -982,7 +1106,7 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -990,7 +1114,7 @@
       <c r="A9" t="s">
         <v>58</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -998,8 +1122,238 @@
       <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A93022-0B83-B54B-BF03-20A27CAE33C8}">
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>